<commit_message>
Trying a different MD parser to fix readme issues on read the docs
</commit_message>
<xml_diff>
--- a/examples/eCommerce_validation_grids.xlsx
+++ b/examples/eCommerce_validation_grids.xlsx
@@ -7446,14 +7446,18 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>38975.66341529859</v>
+        <v>38138.7855310816</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sqrt</t>
+        </is>
+      </c>
       <c r="C3" t="n">
         <v>15</v>
       </c>
@@ -7463,18 +7467,14 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>39444.26741411</v>
+        <v>38347.43130138954</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>sqrt</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
         <v>15</v>
       </c>
@@ -7484,7 +7484,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>40437.39418577377</v>
+        <v>38883.17023023334</v>
       </c>
     </row>
     <row r="5">
@@ -7501,7 +7501,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>41351.3079949142</v>
+        <v>40254.65429963594</v>
       </c>
     </row>
   </sheetData>
@@ -9109,7 +9109,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C2" t="n">
         <v>15</v>
@@ -9120,7 +9120,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>31444.18856391787</v>
+        <v>30617.8858491307</v>
       </c>
     </row>
     <row r="3">
@@ -9128,7 +9128,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C3" t="n">
         <v>15</v>
@@ -9139,7 +9139,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>31567.85395096453</v>
+        <v>31510.53882522551</v>
       </c>
     </row>
     <row r="4">
@@ -9147,7 +9147,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C4" t="n">
         <v>15</v>
@@ -9158,7 +9158,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>31845.82716628566</v>
+        <v>31694.41188994402</v>
       </c>
     </row>
     <row r="5">
@@ -9177,7 +9177,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>33765.21220861652</v>
+        <v>33630.94346143826</v>
       </c>
     </row>
     <row r="6">
@@ -9196,7 +9196,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>33868.04814957009</v>
+        <v>33878.36375391919</v>
       </c>
     </row>
     <row r="7">
@@ -9215,7 +9215,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>35030.40972686402</v>
+        <v>33930.43739896564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed typos in ecommerce notebook
</commit_message>
<xml_diff>
--- a/examples/eCommerce_validation_grids.xlsx
+++ b/examples/eCommerce_validation_grids.xlsx
@@ -58,6 +58,7 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -73,74 +74,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -478,7 +411,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>48871.19624543198</v>
+        <v>48871.19624543202</v>
       </c>
     </row>
     <row r="3">
@@ -496,7 +429,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>48871.1962454321</v>
+        <v>48871.19624543204</v>
       </c>
     </row>
     <row r="4">
@@ -510,7 +443,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>48871.19624543512</v>
+        <v>48871.1962454346</v>
       </c>
     </row>
     <row r="5">
@@ -528,7 +461,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>49292.41029535931</v>
+        <v>49292.41032392419</v>
       </c>
     </row>
   </sheetData>
@@ -603,7 +536,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>28047.22725745376</v>
+        <v>28047.22725745377</v>
       </c>
     </row>
     <row r="3">
@@ -627,7 +560,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>28068.11887294055</v>
+        <v>28068.11887294056</v>
       </c>
     </row>
     <row r="4">
@@ -723,7 +656,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>28178.10948079788</v>
+        <v>28178.1094807979</v>
       </c>
     </row>
     <row r="8">
@@ -771,7 +704,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>28205.40114471167</v>
+        <v>28205.40114471168</v>
       </c>
     </row>
     <row r="10">
@@ -819,7 +752,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>28235.58806258228</v>
+        <v>28235.58806258229</v>
       </c>
     </row>
     <row r="12">
@@ -843,7 +776,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>28257.8942910722</v>
+        <v>28257.89429107221</v>
       </c>
     </row>
     <row r="13">
@@ -867,7 +800,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>28269.15502592365</v>
+        <v>28269.15502592366</v>
       </c>
     </row>
     <row r="14">
@@ -891,7 +824,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>28306.70107959428</v>
+        <v>28306.70107959429</v>
       </c>
     </row>
     <row r="15">
@@ -939,7 +872,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>28348.97517906553</v>
+        <v>28348.97517906554</v>
       </c>
     </row>
     <row r="17">
@@ -987,7 +920,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>28396.92605170628</v>
+        <v>28396.92605170629</v>
       </c>
     </row>
     <row r="19">
@@ -1011,7 +944,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>28431.98293174079</v>
+        <v>28431.9829317408</v>
       </c>
     </row>
     <row r="20">
@@ -1059,7 +992,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>28451.77331580619</v>
+        <v>28451.7733158062</v>
       </c>
     </row>
     <row r="22">
@@ -1083,7 +1016,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>28471.20186317744</v>
+        <v>28471.20186317745</v>
       </c>
     </row>
     <row r="23">
@@ -1107,7 +1040,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>28514.46743529899</v>
+        <v>28514.467435299</v>
       </c>
     </row>
     <row r="24">
@@ -1131,7 +1064,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>28515.11577725342</v>
+        <v>28515.11577725343</v>
       </c>
     </row>
     <row r="25">
@@ -1179,7 +1112,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>28562.4362436333</v>
+        <v>28562.43624363331</v>
       </c>
     </row>
     <row r="27">
@@ -1227,7 +1160,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>28615.91433731918</v>
+        <v>28615.91433731919</v>
       </c>
     </row>
     <row r="29">
@@ -1251,7 +1184,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>28616.88285617072</v>
+        <v>28616.88285617073</v>
       </c>
     </row>
     <row r="30">
@@ -1299,7 +1232,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>28676.54939413795</v>
+        <v>28676.54939413796</v>
       </c>
     </row>
     <row r="32">
@@ -1323,7 +1256,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>28743.65653075243</v>
+        <v>28743.65653075244</v>
       </c>
     </row>
     <row r="33">
@@ -1347,7 +1280,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>28744.60399441605</v>
+        <v>28744.60399441606</v>
       </c>
     </row>
     <row r="34">
@@ -1371,7 +1304,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>28781.55891991594</v>
+        <v>28781.55891991595</v>
       </c>
     </row>
     <row r="35">
@@ -1443,7 +1376,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>28909.93867275364</v>
+        <v>28909.93867275365</v>
       </c>
     </row>
     <row r="38">
@@ -1491,7 +1424,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>29012.01613259136</v>
+        <v>29012.01613259137</v>
       </c>
     </row>
     <row r="40">
@@ -1515,7 +1448,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>29070.39285277082</v>
+        <v>29070.39285277083</v>
       </c>
     </row>
     <row r="41">
@@ -1539,7 +1472,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>29130.65120398339</v>
+        <v>29130.6512039834</v>
       </c>
     </row>
     <row r="42">
@@ -1587,7 +1520,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>29133.46637826232</v>
+        <v>29133.46637826233</v>
       </c>
     </row>
     <row r="44">
@@ -1659,7 +1592,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>29275.89203784668</v>
+        <v>29275.8920378467</v>
       </c>
     </row>
     <row r="47">
@@ -1683,7 +1616,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>29276.51653752886</v>
+        <v>29276.51653752887</v>
       </c>
     </row>
     <row r="48">
@@ -1707,7 +1640,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>29356.38422195082</v>
+        <v>29356.38422195083</v>
       </c>
     </row>
     <row r="49">
@@ -1731,7 +1664,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>29447.34692322275</v>
+        <v>29447.34692322276</v>
       </c>
     </row>
     <row r="50">
@@ -1923,7 +1856,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>29930.86105165588</v>
+        <v>29930.86105165589</v>
       </c>
     </row>
     <row r="58">
@@ -1995,7 +1928,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>29933.6174660449</v>
+        <v>29933.61746604491</v>
       </c>
     </row>
     <row r="61">
@@ -2019,7 +1952,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>30094.19761841322</v>
+        <v>30094.19761841323</v>
       </c>
     </row>
     <row r="62">
@@ -2187,7 +2120,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>30761.02831923076</v>
+        <v>30761.02831923077</v>
       </c>
     </row>
     <row r="69">
@@ -2379,7 +2312,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>32513.78833405797</v>
+        <v>32513.78833405798</v>
       </c>
     </row>
     <row r="77">
@@ -2499,7 +2432,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>36558.91275704366</v>
+        <v>36558.91275704367</v>
       </c>
     </row>
     <row r="82">
@@ -2547,7 +2480,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>37028.45698895315</v>
+        <v>37028.45698895313</v>
       </c>
     </row>
     <row r="84">
@@ -2571,7 +2504,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>37248.19963774404</v>
+        <v>37248.19963774407</v>
       </c>
     </row>
     <row r="85">
@@ -2595,7 +2528,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>37479.24742131651</v>
+        <v>37479.24742131653</v>
       </c>
     </row>
     <row r="86">
@@ -2619,7 +2552,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>37722.63521625992</v>
+        <v>37722.63521625991</v>
       </c>
     </row>
     <row r="87">
@@ -2643,7 +2576,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>37978.19973881627</v>
+        <v>37978.19973881628</v>
       </c>
     </row>
     <row r="88">
@@ -2667,7 +2600,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>37979.55457875325</v>
+        <v>37979.55457875331</v>
       </c>
     </row>
     <row r="89">
@@ -2691,7 +2624,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>38180.62900682498</v>
+        <v>38180.62900682499</v>
       </c>
     </row>
     <row r="90">
@@ -2715,7 +2648,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>38251.39014261474</v>
+        <v>38251.39014261472</v>
       </c>
     </row>
     <row r="91">
@@ -2835,7 +2768,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>38846.62122543864</v>
+        <v>38846.62122543867</v>
       </c>
     </row>
     <row r="96">
@@ -2859,7 +2792,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>39089.10382740397</v>
+        <v>39089.10382740399</v>
       </c>
     </row>
     <row r="97">
@@ -2883,7 +2816,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>39174.28098158046</v>
+        <v>39174.28098158051</v>
       </c>
     </row>
     <row r="98">
@@ -2907,7 +2840,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>39345.65716937991</v>
+        <v>39345.65716937993</v>
       </c>
     </row>
     <row r="99">
@@ -2931,7 +2864,7 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>39522.16175480282</v>
+        <v>39522.16175480283</v>
       </c>
     </row>
     <row r="100">
@@ -2955,7 +2888,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>39525.60601036808</v>
+        <v>39525.6060103681</v>
       </c>
     </row>
     <row r="101">
@@ -3003,7 +2936,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>39707.82512837352</v>
+        <v>39707.82512837353</v>
       </c>
     </row>
     <row r="103">
@@ -3027,7 +2960,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>39900.87082749646</v>
+        <v>39900.87082749647</v>
       </c>
     </row>
     <row r="104">
@@ -3051,7 +2984,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>39903.07378518595</v>
+        <v>39903.07378518597</v>
       </c>
     </row>
     <row r="105">
@@ -3075,7 +3008,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>39904.17307059006</v>
+        <v>39904.17307059009</v>
       </c>
     </row>
     <row r="106">
@@ -3099,7 +3032,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>40101.85443707079</v>
+        <v>40101.8544370708</v>
       </c>
     </row>
     <row r="107">
@@ -3147,7 +3080,7 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>40311.47224775816</v>
+        <v>40311.47224775817</v>
       </c>
     </row>
     <row r="109">
@@ -3171,7 +3104,7 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>40314.56684896955</v>
+        <v>40314.56684896967</v>
       </c>
     </row>
     <row r="110">
@@ -3195,7 +3128,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>40530.53001825057</v>
+        <v>40530.5300182506</v>
       </c>
     </row>
     <row r="111">
@@ -3243,7 +3176,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>40759.96915471624</v>
+        <v>40759.96915471625</v>
       </c>
     </row>
     <row r="113">
@@ -3267,7 +3200,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>40762.84093296405</v>
+        <v>40762.84093296408</v>
       </c>
     </row>
     <row r="114">
@@ -3291,7 +3224,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>40880.80212858244</v>
+        <v>40880.80212858245</v>
       </c>
     </row>
     <row r="115">
@@ -3315,7 +3248,7 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>41000.90178435899</v>
+        <v>41000.901784359</v>
       </c>
     </row>
     <row r="116">
@@ -3339,7 +3272,7 @@
         </is>
       </c>
       <c r="F116" t="n">
-        <v>41254.65020359327</v>
+        <v>41254.65020359329</v>
       </c>
     </row>
     <row r="117">
@@ -3363,7 +3296,7 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>41256.4147470447</v>
+        <v>41256.41474704471</v>
       </c>
     </row>
     <row r="118">
@@ -3387,7 +3320,7 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>41257.29022547129</v>
+        <v>41257.29022547131</v>
       </c>
     </row>
     <row r="119">
@@ -3411,7 +3344,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>41522.84801158925</v>
+        <v>41522.84801158927</v>
       </c>
     </row>
     <row r="120">
@@ -3435,7 +3368,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>41664.59191292801</v>
+        <v>41664.59191292803</v>
       </c>
     </row>
     <row r="121">
@@ -3459,7 +3392,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>41802.69324089872</v>
+        <v>41802.69324089874</v>
       </c>
     </row>
     <row r="122">
@@ -3483,7 +3416,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>41807.46466344338</v>
+        <v>41807.4646634434</v>
       </c>
     </row>
     <row r="123">
@@ -3507,7 +3440,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>41809.83275530805</v>
+        <v>41809.832755308</v>
       </c>
     </row>
     <row r="124">
@@ -3531,7 +3464,7 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>41952.21161324761</v>
+        <v>41952.21161324763</v>
       </c>
     </row>
     <row r="125">
@@ -3555,7 +3488,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>42106.74005831934</v>
+        <v>42106.74005831935</v>
       </c>
     </row>
     <row r="126">
@@ -3579,7 +3512,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>42111.07598433988</v>
+        <v>42111.0759843399</v>
       </c>
     </row>
     <row r="127">
@@ -3603,7 +3536,7 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>42112.50609370896</v>
+        <v>42112.50609370898</v>
       </c>
     </row>
     <row r="128">
@@ -3627,7 +3560,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>42266.7088167066</v>
+        <v>42266.70881670662</v>
       </c>
     </row>
     <row r="129">
@@ -3651,7 +3584,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>42432.65607086133</v>
+        <v>42432.65607086135</v>
       </c>
     </row>
     <row r="130">
@@ -3675,7 +3608,7 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>42436.70389849861</v>
+        <v>42436.70389849863</v>
       </c>
     </row>
     <row r="131">
@@ -3699,7 +3632,7 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>42438.70053567944</v>
+        <v>42438.70053567949</v>
       </c>
     </row>
     <row r="132">
@@ -3723,7 +3656,7 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>42605.18197450334</v>
+        <v>42605.18197450336</v>
       </c>
     </row>
     <row r="133">
@@ -3747,7 +3680,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>42610.35481831271</v>
+        <v>42610.35481831273</v>
       </c>
     </row>
     <row r="134">
@@ -3771,7 +3704,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>42784.91805994082</v>
+        <v>42784.91805994084</v>
       </c>
     </row>
     <row r="135">
@@ -3795,7 +3728,7 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>42788.65146761524</v>
+        <v>42788.65146761526</v>
       </c>
     </row>
     <row r="136">
@@ -3819,7 +3752,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>42972.63323431753</v>
+        <v>42972.63323431755</v>
       </c>
     </row>
     <row r="137">
@@ -3843,7 +3776,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>43169.24080588189</v>
+        <v>43169.24080588191</v>
       </c>
     </row>
     <row r="138">
@@ -3867,7 +3800,7 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>43172.65255807369</v>
+        <v>43172.65255807371</v>
       </c>
     </row>
     <row r="139">
@@ -3891,7 +3824,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>43173.77361796163</v>
+        <v>43173.77361796165</v>
       </c>
     </row>
     <row r="140">
@@ -3915,7 +3848,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>43174.33339491871</v>
+        <v>43174.33339491872</v>
       </c>
     </row>
     <row r="141">
@@ -3939,7 +3872,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>43375.70843080634</v>
+        <v>43375.70843080636</v>
       </c>
     </row>
     <row r="142">
@@ -3963,7 +3896,7 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>43593.40498610504</v>
+        <v>43593.40498610506</v>
       </c>
     </row>
     <row r="143">
@@ -3987,7 +3920,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>43596.73206487506</v>
+        <v>43596.73206487509</v>
       </c>
     </row>
     <row r="144">
@@ -4011,7 +3944,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>43825.41813334785</v>
+        <v>43825.41813334787</v>
       </c>
     </row>
     <row r="145">
@@ -4035,7 +3968,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>43828.6709947827</v>
+        <v>43828.67099478273</v>
       </c>
     </row>
     <row r="146">
@@ -4059,7 +3992,7 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>44071.78144094747</v>
+        <v>44071.78144094749</v>
       </c>
     </row>
     <row r="147">
@@ -4083,7 +4016,7 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>44073.89997799744</v>
+        <v>44073.89997799746</v>
       </c>
     </row>
     <row r="148">
@@ -4107,7 +4040,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>44074.93561189927</v>
+        <v>44074.93561189922</v>
       </c>
     </row>
     <row r="149">
@@ -4131,7 +4064,7 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>44335.89034912773</v>
+        <v>44335.89034912776</v>
       </c>
     </row>
     <row r="150">
@@ -4155,7 +4088,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>44621.87769917012</v>
+        <v>44621.87769917014</v>
       </c>
     </row>
     <row r="151">
@@ -4179,7 +4112,7 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>44623.64109675361</v>
+        <v>44623.64109675363</v>
       </c>
     </row>
     <row r="152">
@@ -4203,7 +4136,7 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>44624.22128147935</v>
+        <v>44624.22128147937</v>
       </c>
     </row>
     <row r="153">
@@ -4227,7 +4160,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>44935.44432508935</v>
+        <v>44935.44432508938</v>
       </c>
     </row>
     <row r="154">
@@ -4251,7 +4184,7 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>45285.68672718328</v>
+        <v>45285.68672718332</v>
       </c>
     </row>
     <row r="155">
@@ -4275,7 +4208,7 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>45287.06602002272</v>
+        <v>45287.06602002276</v>
       </c>
     </row>
     <row r="156">
@@ -4299,7 +4232,7 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>45287.74717618968</v>
+        <v>45287.74717618978</v>
       </c>
     </row>
     <row r="157">
@@ -4323,7 +4256,7 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>45689.26979913766</v>
+        <v>45689.26979913768</v>
       </c>
     </row>
     <row r="158">
@@ -4347,7 +4280,7 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>45690.81790576928</v>
+        <v>45690.81790576931</v>
       </c>
     </row>
     <row r="159">
@@ -4371,7 +4304,7 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>46184.07453892759</v>
+        <v>46184.07453892761</v>
       </c>
     </row>
     <row r="160">
@@ -4395,7 +4328,7 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>46185.03299580719</v>
+        <v>46185.03299580723</v>
       </c>
     </row>
     <row r="161">
@@ -4419,7 +4352,7 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>46894.72163987394</v>
+        <v>46894.72163987396</v>
       </c>
     </row>
     <row r="162">
@@ -4443,7 +4376,7 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>48623.81223883682</v>
+        <v>48623.81223883681</v>
       </c>
     </row>
     <row r="163">
@@ -4467,7 +4400,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>48634.68362459853</v>
+        <v>48634.68362459849</v>
       </c>
     </row>
     <row r="164">
@@ -4491,7 +4424,7 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>48645.72636084372</v>
+        <v>48645.7263608438</v>
       </c>
     </row>
     <row r="165">
@@ -4539,7 +4472,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>48677.95901759185</v>
+        <v>48677.95901759194</v>
       </c>
     </row>
     <row r="167">
@@ -4563,7 +4496,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>48698.81326677007</v>
+        <v>48698.81326677011</v>
       </c>
     </row>
     <row r="168">
@@ -4587,7 +4520,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>48719.69365913058</v>
+        <v>48719.69365913055</v>
       </c>
     </row>
     <row r="169">
@@ -4611,7 +4544,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>48740.60186821026</v>
+        <v>48740.60186821027</v>
       </c>
     </row>
     <row r="170">
@@ -4635,7 +4568,7 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>48750.00461913754</v>
+        <v>48750.00461913757</v>
       </c>
     </row>
     <row r="171">
@@ -4659,7 +4592,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>48758.76923307505</v>
+        <v>48758.76923307506</v>
       </c>
     </row>
     <row r="172">
@@ -4683,7 +4616,7 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>48767.90846865263</v>
+        <v>48767.90846865268</v>
       </c>
     </row>
     <row r="173">
@@ -4707,7 +4640,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>48777.47026227123</v>
+        <v>48777.47026227129</v>
       </c>
     </row>
     <row r="174">
@@ -4731,7 +4664,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>48787.47048877252</v>
+        <v>48787.47048877254</v>
       </c>
     </row>
     <row r="175">
@@ -4755,7 +4688,7 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>48797.88861425842</v>
+        <v>48797.88861425844</v>
       </c>
     </row>
     <row r="176">
@@ -4799,7 +4732,7 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>48809.70484376087</v>
+        <v>48809.70484376088</v>
       </c>
     </row>
     <row r="178">
@@ -4819,7 +4752,7 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>48812.75792393344</v>
+        <v>48812.75792393342</v>
       </c>
     </row>
     <row r="179">
@@ -4839,7 +4772,7 @@
         </is>
       </c>
       <c r="F179" t="n">
-        <v>48815.81339962385</v>
+        <v>48815.81339962389</v>
       </c>
     </row>
     <row r="180">
@@ -4879,7 +4812,7 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>48821.93153713351</v>
+        <v>48821.93153713353</v>
       </c>
     </row>
     <row r="182">
@@ -4899,7 +4832,7 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>48824.99419700116</v>
+        <v>48824.99419700122</v>
       </c>
     </row>
     <row r="183">
@@ -4919,7 +4852,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>48828.05925045699</v>
+        <v>48828.05925045704</v>
       </c>
     </row>
     <row r="184">
@@ -4939,7 +4872,7 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>48831.12669718039</v>
+        <v>48831.1266971804</v>
       </c>
     </row>
     <row r="185">
@@ -4963,7 +4896,7 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>48831.64765154054</v>
+        <v>48831.6476515406</v>
       </c>
     </row>
     <row r="186">
@@ -4983,7 +4916,7 @@
         </is>
       </c>
       <c r="F186" t="n">
-        <v>48834.19653738203</v>
+        <v>48834.19653738209</v>
       </c>
     </row>
     <row r="187">
@@ -5003,7 +4936,7 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>48837.26877025461</v>
+        <v>48837.26877025455</v>
       </c>
     </row>
     <row r="188">
@@ -5023,7 +4956,7 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>48840.34339504584</v>
+        <v>48840.34339504587</v>
       </c>
     </row>
     <row r="189">
@@ -5043,7 +4976,7 @@
         </is>
       </c>
       <c r="F189" t="n">
-        <v>48843.4204105587</v>
+        <v>48843.42041055865</v>
       </c>
     </row>
     <row r="190">
@@ -5067,7 +5000,7 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>48845.72337023898</v>
+        <v>48845.723370239</v>
       </c>
     </row>
     <row r="191">
@@ -5087,7 +5020,7 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>48846.4998170473</v>
+        <v>48846.49981704731</v>
       </c>
     </row>
     <row r="192">
@@ -5107,7 +5040,7 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>48849.58161504691</v>
+        <v>48849.58161504694</v>
       </c>
     </row>
     <row r="193">
@@ -5131,7 +5064,7 @@
         </is>
       </c>
       <c r="F193" t="n">
-        <v>48849.64390232728</v>
+        <v>48849.64390232731</v>
       </c>
     </row>
     <row r="194">
@@ -5151,7 +5084,7 @@
         </is>
       </c>
       <c r="F194" t="n">
-        <v>48852.66580318245</v>
+        <v>48852.66580318239</v>
       </c>
     </row>
     <row r="195">
@@ -5195,7 +5128,7 @@
         </is>
       </c>
       <c r="F196" t="n">
-        <v>48855.75238097481</v>
+        <v>48855.75238097482</v>
       </c>
     </row>
     <row r="197">
@@ -5219,7 +5152,7 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>48857.51433129699</v>
+        <v>48857.514331297</v>
       </c>
     </row>
     <row r="198">
@@ -5243,7 +5176,7 @@
         </is>
       </c>
       <c r="F198" t="n">
-        <v>48857.62701671276</v>
+        <v>48857.62701671277</v>
       </c>
     </row>
     <row r="199">
@@ -5263,7 +5196,7 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>48858.84134786957</v>
+        <v>48858.84134786958</v>
       </c>
     </row>
     <row r="200">
@@ -5287,7 +5220,7 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>48859.48131515855</v>
+        <v>48859.48131515858</v>
       </c>
     </row>
     <row r="201">
@@ -5335,7 +5268,7 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>48860.98160043218</v>
+        <v>48860.9816004322</v>
       </c>
     </row>
     <row r="203">
@@ -5359,7 +5292,7 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>48861.69077039745</v>
+        <v>48861.69077039748</v>
       </c>
     </row>
     <row r="204">
@@ -5379,7 +5312,7 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>48861.93270313048</v>
+        <v>48861.93270313042</v>
       </c>
     </row>
     <row r="205">
@@ -5403,7 +5336,7 @@
         </is>
       </c>
       <c r="F205" t="n">
-        <v>48862.40026698034</v>
+        <v>48862.40026698033</v>
       </c>
     </row>
     <row r="206">
@@ -5451,7 +5384,7 @@
         </is>
       </c>
       <c r="F207" t="n">
-        <v>48863.82804121597</v>
+        <v>48863.828041216</v>
       </c>
     </row>
     <row r="208">
@@ -5475,7 +5408,7 @@
         </is>
       </c>
       <c r="F208" t="n">
-        <v>48864.54287044584</v>
+        <v>48864.54287044583</v>
       </c>
     </row>
     <row r="209">
@@ -5495,7 +5428,7 @@
         </is>
       </c>
       <c r="F209" t="n">
-        <v>48865.0264473741</v>
+        <v>48865.02644737406</v>
       </c>
     </row>
     <row r="210">
@@ -5519,7 +5452,7 @@
         </is>
       </c>
       <c r="F210" t="n">
-        <v>48865.2614431929</v>
+        <v>48865.26144319287</v>
       </c>
     </row>
     <row r="211">
@@ -5543,7 +5476,7 @@
         </is>
       </c>
       <c r="F211" t="n">
-        <v>48865.98608390537</v>
+        <v>48865.98608390542</v>
       </c>
     </row>
     <row r="212">
@@ -5567,7 +5500,7 @@
         </is>
       </c>
       <c r="F212" t="n">
-        <v>48866.7189184861</v>
+        <v>48866.71891848611</v>
       </c>
     </row>
     <row r="213">
@@ -5591,7 +5524,7 @@
         </is>
       </c>
       <c r="F213" t="n">
-        <v>48867.45183191235</v>
+        <v>48867.45183191234</v>
       </c>
     </row>
     <row r="214">
@@ -5611,7 +5544,7 @@
         </is>
       </c>
       <c r="F214" t="n">
-        <v>48868.12257946286</v>
+        <v>48868.12257946288</v>
       </c>
     </row>
     <row r="215">
@@ -5659,7 +5592,7 @@
         </is>
       </c>
       <c r="F216" t="n">
-        <v>48868.93495464877</v>
+        <v>48868.93495464883</v>
       </c>
     </row>
     <row r="217">
@@ -5683,7 +5616,7 @@
         </is>
       </c>
       <c r="F217" t="n">
-        <v>48869.68394805572</v>
+        <v>48869.6839480558</v>
       </c>
     </row>
     <row r="218">
@@ -5707,7 +5640,7 @@
         </is>
       </c>
       <c r="F218" t="n">
-        <v>48870.43721491363</v>
+        <v>48870.4372149136</v>
       </c>
     </row>
     <row r="219">
@@ -5731,7 +5664,7 @@
         </is>
       </c>
       <c r="F219" t="n">
-        <v>48871.02755204459</v>
+        <v>48871.02755204464</v>
       </c>
     </row>
     <row r="220">
@@ -5755,7 +5688,7 @@
         </is>
       </c>
       <c r="F220" t="n">
-        <v>48873.45596961863</v>
+        <v>48873.45596961867</v>
       </c>
     </row>
     <row r="221">
@@ -5779,7 +5712,7 @@
         </is>
       </c>
       <c r="F221" t="n">
-        <v>48876.54624803982</v>
+        <v>48876.54624803981</v>
       </c>
     </row>
     <row r="222">
@@ -5819,7 +5752,7 @@
         </is>
       </c>
       <c r="F223" t="n">
-        <v>49506.25077896447</v>
+        <v>49506.25077896452</v>
       </c>
     </row>
     <row r="224">
@@ -5839,7 +5772,7 @@
         </is>
       </c>
       <c r="F224" t="n">
-        <v>49506.33750832998</v>
+        <v>49506.33750833001</v>
       </c>
     </row>
     <row r="225">
@@ -5859,7 +5792,7 @@
         </is>
       </c>
       <c r="F225" t="n">
-        <v>49736.24997676902</v>
+        <v>49736.24997676903</v>
       </c>
     </row>
     <row r="226">
@@ -5899,7 +5832,7 @@
         </is>
       </c>
       <c r="F227" t="n">
-        <v>49888.80553299074</v>
+        <v>49888.80553299079</v>
       </c>
     </row>
     <row r="228">
@@ -5919,7 +5852,7 @@
         </is>
       </c>
       <c r="F228" t="n">
-        <v>49888.87368359465</v>
+        <v>49888.87368359471</v>
       </c>
     </row>
     <row r="229">
@@ -5939,7 +5872,7 @@
         </is>
       </c>
       <c r="F229" t="n">
-        <v>49889.0100277433</v>
+        <v>49889.01002774332</v>
       </c>
     </row>
     <row r="230">
@@ -5959,7 +5892,7 @@
         </is>
       </c>
       <c r="F230" t="n">
-        <v>49998.78499281825</v>
+        <v>49998.78499281831</v>
       </c>
     </row>
     <row r="231">
@@ -5979,7 +5912,7 @@
         </is>
       </c>
       <c r="F231" t="n">
-        <v>50080.52352988078</v>
+        <v>50080.5235298808</v>
       </c>
     </row>
     <row r="232">
@@ -5999,7 +5932,7 @@
         </is>
       </c>
       <c r="F232" t="n">
-        <v>50080.6900259711</v>
+        <v>50080.69002597107</v>
       </c>
     </row>
     <row r="233">
@@ -6019,7 +5952,7 @@
         </is>
       </c>
       <c r="F233" t="n">
-        <v>50081.1895751515</v>
+        <v>50081.18957515149</v>
       </c>
     </row>
     <row r="234">
@@ -6039,7 +5972,7 @@
         </is>
       </c>
       <c r="F234" t="n">
-        <v>50145.59252304758</v>
+        <v>50145.59252304768</v>
       </c>
     </row>
     <row r="235">
@@ -6059,7 +5992,7 @@
         </is>
       </c>
       <c r="F235" t="n">
-        <v>50196.51564995847</v>
+        <v>50196.51564995854</v>
       </c>
     </row>
     <row r="236">
@@ -6079,7 +6012,7 @@
         </is>
       </c>
       <c r="F236" t="n">
-        <v>50196.79216974838</v>
+        <v>50196.79216974836</v>
       </c>
     </row>
     <row r="237">
@@ -6099,7 +6032,7 @@
         </is>
       </c>
       <c r="F237" t="n">
-        <v>50197.3452874842</v>
+        <v>50197.34528748424</v>
       </c>
     </row>
     <row r="238">
@@ -6119,7 +6052,7 @@
         </is>
       </c>
       <c r="F238" t="n">
-        <v>50239.09316529176</v>
+        <v>50239.09316529177</v>
       </c>
     </row>
     <row r="239">
@@ -6139,7 +6072,7 @@
         </is>
       </c>
       <c r="F239" t="n">
-        <v>50239.85721479142</v>
+        <v>50239.8572147915</v>
       </c>
     </row>
     <row r="240">
@@ -6159,7 +6092,7 @@
         </is>
       </c>
       <c r="F240" t="n">
-        <v>50274.81845828815</v>
+        <v>50274.81845828814</v>
       </c>
     </row>
     <row r="241">
@@ -6179,7 +6112,7 @@
         </is>
       </c>
       <c r="F241" t="n">
-        <v>50275.40832874496</v>
+        <v>50275.408328745</v>
       </c>
     </row>
     <row r="242">
@@ -6199,7 +6132,7 @@
         </is>
       </c>
       <c r="F242" t="n">
-        <v>50305.58321229229</v>
+        <v>50305.58321229231</v>
       </c>
     </row>
     <row r="243">
@@ -6219,7 +6152,7 @@
         </is>
       </c>
       <c r="F243" t="n">
-        <v>50330.59325892073</v>
+        <v>50330.59325892078</v>
       </c>
     </row>
     <row r="244">
@@ -6239,7 +6172,7 @@
         </is>
       </c>
       <c r="F244" t="n">
-        <v>50330.69602334152</v>
+        <v>50330.69602334149</v>
       </c>
     </row>
     <row r="245">
@@ -6259,7 +6192,7 @@
         </is>
       </c>
       <c r="F245" t="n">
-        <v>50330.90156220426</v>
+        <v>50330.9015622043</v>
       </c>
     </row>
     <row r="246">
@@ -6279,7 +6212,7 @@
         </is>
       </c>
       <c r="F246" t="n">
-        <v>50331.51825896248</v>
+        <v>50331.51825896251</v>
       </c>
     </row>
     <row r="247">
@@ -6299,7 +6232,7 @@
         </is>
       </c>
       <c r="F247" t="n">
-        <v>50354.05007759432</v>
+        <v>50354.05007759434</v>
       </c>
     </row>
     <row r="248">
@@ -6319,7 +6252,7 @@
         </is>
       </c>
       <c r="F248" t="n">
-        <v>50373.17124651623</v>
+        <v>50373.17124651624</v>
       </c>
     </row>
     <row r="249">
@@ -6339,7 +6272,7 @@
         </is>
       </c>
       <c r="F249" t="n">
-        <v>50373.80843082751</v>
+        <v>50373.8084308275</v>
       </c>
     </row>
     <row r="250">
@@ -6359,7 +6292,7 @@
         </is>
       </c>
       <c r="F250" t="n">
-        <v>50390.41560118299</v>
+        <v>50390.41560118301</v>
       </c>
     </row>
     <row r="251">
@@ -6379,7 +6312,7 @@
         </is>
       </c>
       <c r="F251" t="n">
-        <v>50391.27654184485</v>
+        <v>50391.27654184483</v>
       </c>
     </row>
     <row r="252">
@@ -6399,7 +6332,7 @@
         </is>
       </c>
       <c r="F252" t="n">
-        <v>50405.85140765616</v>
+        <v>50405.85140765615</v>
       </c>
     </row>
     <row r="253">
@@ -6419,7 +6352,7 @@
         </is>
       </c>
       <c r="F253" t="n">
-        <v>50406.17804845503</v>
+        <v>50406.17804845506</v>
       </c>
     </row>
     <row r="254">
@@ -6439,7 +6372,7 @@
         </is>
       </c>
       <c r="F254" t="n">
-        <v>50406.83142762403</v>
+        <v>50406.83142762411</v>
       </c>
     </row>
     <row r="255">
@@ -6459,7 +6392,7 @@
         </is>
       </c>
       <c r="F255" t="n">
-        <v>50420.77158701097</v>
+        <v>50420.77158701098</v>
       </c>
     </row>
     <row r="256">
@@ -6479,7 +6412,7 @@
         </is>
       </c>
       <c r="F256" t="n">
-        <v>50432.44776722284</v>
+        <v>50432.44776722287</v>
       </c>
     </row>
     <row r="257">
@@ -6499,7 +6432,7 @@
         </is>
       </c>
       <c r="F257" t="n">
-        <v>50432.66991467409</v>
+        <v>50432.66991467408</v>
       </c>
     </row>
     <row r="258">
@@ -6519,7 +6452,7 @@
         </is>
       </c>
       <c r="F258" t="n">
-        <v>50433.33644621748</v>
+        <v>50433.33644621752</v>
       </c>
     </row>
     <row r="259">
@@ -6539,7 +6472,7 @@
         </is>
       </c>
       <c r="F259" t="n">
-        <v>50444.72029275002</v>
+        <v>50444.72029275005</v>
       </c>
     </row>
     <row r="260">
@@ -6559,7 +6492,7 @@
         </is>
       </c>
       <c r="F260" t="n">
-        <v>50454.06631956046</v>
+        <v>50454.06631956044</v>
       </c>
     </row>
     <row r="261">
@@ -6579,7 +6512,7 @@
         </is>
       </c>
       <c r="F261" t="n">
-        <v>50454.40499213691</v>
+        <v>50454.40499213689</v>
       </c>
     </row>
     <row r="262">
@@ -6599,7 +6532,7 @@
         </is>
       </c>
       <c r="F262" t="n">
-        <v>50455.08243999176</v>
+        <v>50455.08243999177</v>
       </c>
     </row>
     <row r="263">
@@ -6639,7 +6572,7 @@
         </is>
       </c>
       <c r="F264" t="n">
-        <v>50472.56068702526</v>
+        <v>50472.56068702523</v>
       </c>
     </row>
     <row r="265">
@@ -6659,7 +6592,7 @@
         </is>
       </c>
       <c r="F265" t="n">
-        <v>50487.6080071336</v>
+        <v>50487.60800713365</v>
       </c>
     </row>
     <row r="266">
@@ -6679,7 +6612,7 @@
         </is>
       </c>
       <c r="F266" t="n">
-        <v>50487.7237490607</v>
+        <v>50487.72374906072</v>
       </c>
     </row>
     <row r="267">
@@ -6699,7 +6632,7 @@
         </is>
       </c>
       <c r="F267" t="n">
-        <v>50487.95524475581</v>
+        <v>50487.95524475587</v>
       </c>
     </row>
     <row r="268">
@@ -6719,7 +6652,7 @@
         </is>
       </c>
       <c r="F268" t="n">
-        <v>50501.17503544766</v>
+        <v>50501.17503544771</v>
       </c>
     </row>
     <row r="269">
@@ -6739,7 +6672,7 @@
         </is>
       </c>
       <c r="F269" t="n">
-        <v>50506.87393600326</v>
+        <v>50506.87393600325</v>
       </c>
     </row>
     <row r="270">
@@ -6759,7 +6692,7 @@
         </is>
       </c>
       <c r="F270" t="n">
-        <v>50512.29759010938</v>
+        <v>50512.29759010943</v>
       </c>
     </row>
     <row r="271">
@@ -6779,7 +6712,7 @@
         </is>
       </c>
       <c r="F271" t="n">
-        <v>50512.65127716726</v>
+        <v>50512.65127716729</v>
       </c>
     </row>
     <row r="272">
@@ -6799,7 +6732,7 @@
         </is>
       </c>
       <c r="F272" t="n">
-        <v>50522.47060385872</v>
+        <v>50522.47060385875</v>
       </c>
     </row>
     <row r="273">
@@ -6819,7 +6752,7 @@
         </is>
       </c>
       <c r="F273" t="n">
-        <v>50522.70818069332</v>
+        <v>50522.70818069333</v>
       </c>
     </row>
     <row r="274">
@@ -6859,7 +6792,7 @@
         </is>
       </c>
       <c r="F275" t="n">
-        <v>50531.59421155182</v>
+        <v>50531.59421155187</v>
       </c>
     </row>
     <row r="276">
@@ -6879,7 +6812,7 @@
         </is>
       </c>
       <c r="F276" t="n">
-        <v>50535.42047146213</v>
+        <v>50535.42047146215</v>
       </c>
     </row>
     <row r="277">
@@ -6919,7 +6852,7 @@
         </is>
       </c>
       <c r="F278" t="n">
-        <v>50546.22482193114</v>
+        <v>50546.22482193113</v>
       </c>
     </row>
     <row r="279">
@@ -6939,7 +6872,7 @@
         </is>
       </c>
       <c r="F279" t="n">
-        <v>50546.34576476762</v>
+        <v>50546.34576476763</v>
       </c>
     </row>
     <row r="280">
@@ -6959,7 +6892,7 @@
         </is>
       </c>
       <c r="F280" t="n">
-        <v>50546.58766315414</v>
+        <v>50546.58766315417</v>
       </c>
     </row>
     <row r="281">
@@ -6979,7 +6912,7 @@
         </is>
       </c>
       <c r="F281" t="n">
-        <v>50552.97091148287</v>
+        <v>50552.97091148289</v>
       </c>
     </row>
     <row r="282">
@@ -6999,7 +6932,7 @@
         </is>
       </c>
       <c r="F282" t="n">
-        <v>50555.68770844512</v>
+        <v>50555.68770844516</v>
       </c>
     </row>
     <row r="283">
@@ -7039,7 +6972,7 @@
         </is>
       </c>
       <c r="F284" t="n">
-        <v>50558.75221157004</v>
+        <v>50558.75221157003</v>
       </c>
     </row>
     <row r="285">
@@ -7059,7 +6992,7 @@
         </is>
       </c>
       <c r="F285" t="n">
-        <v>50563.76789900374</v>
+        <v>50563.76789900378</v>
       </c>
     </row>
     <row r="286">
@@ -7079,7 +7012,7 @@
         </is>
       </c>
       <c r="F286" t="n">
-        <v>50568.45174187645</v>
+        <v>50568.45174187647</v>
       </c>
     </row>
     <row r="287">
@@ -7099,7 +7032,7 @@
         </is>
       </c>
       <c r="F287" t="n">
-        <v>50570.82628841423</v>
+        <v>50570.82628841426</v>
       </c>
     </row>
     <row r="288">
@@ -7139,7 +7072,7 @@
         </is>
       </c>
       <c r="F289" t="n">
-        <v>50577.04555723938</v>
+        <v>50577.04555723943</v>
       </c>
     </row>
     <row r="290">
@@ -7159,7 +7092,7 @@
         </is>
       </c>
       <c r="F290" t="n">
-        <v>50582.56724684417</v>
+        <v>50582.56724684415</v>
       </c>
     </row>
     <row r="291">
@@ -7179,7 +7112,7 @@
         </is>
       </c>
       <c r="F291" t="n">
-        <v>50584.14817726918</v>
+        <v>50584.14817726924</v>
       </c>
     </row>
     <row r="292">
@@ -7199,7 +7132,7 @@
         </is>
       </c>
       <c r="F292" t="n">
-        <v>50587.50272833369</v>
+        <v>50587.50272833372</v>
       </c>
     </row>
     <row r="293">
@@ -7219,7 +7152,7 @@
         </is>
       </c>
       <c r="F293" t="n">
-        <v>50590.38679404208</v>
+        <v>50590.38679404209</v>
       </c>
     </row>
     <row r="294">
@@ -7259,7 +7192,7 @@
         </is>
       </c>
       <c r="F295" t="n">
-        <v>50595.82753819307</v>
+        <v>50595.82753819312</v>
       </c>
     </row>
     <row r="296">
@@ -7279,7 +7212,7 @@
         </is>
       </c>
       <c r="F296" t="n">
-        <v>50595.93848926794</v>
+        <v>50595.93848926797</v>
       </c>
     </row>
     <row r="297">
@@ -7299,7 +7232,7 @@
         </is>
       </c>
       <c r="F297" t="n">
-        <v>50600.61456551451</v>
+        <v>50600.61456551454</v>
       </c>
     </row>
     <row r="298">
@@ -7319,7 +7252,7 @@
         </is>
       </c>
       <c r="F298" t="n">
-        <v>50604.85924248766</v>
+        <v>50604.85924248768</v>
       </c>
     </row>
     <row r="299">
@@ -7339,7 +7272,7 @@
         </is>
       </c>
       <c r="F299" t="n">
-        <v>50608.64897280908</v>
+        <v>50608.64897280907</v>
       </c>
     </row>
     <row r="300">
@@ -7359,7 +7292,7 @@
         </is>
       </c>
       <c r="F300" t="n">
-        <v>50612.05331740466</v>
+        <v>50612.05331740469</v>
       </c>
     </row>
     <row r="301">
@@ -7379,7 +7312,7 @@
         </is>
       </c>
       <c r="F301" t="n">
-        <v>50615.12832927346</v>
+        <v>50615.12832927353</v>
       </c>
     </row>
   </sheetData>
@@ -7446,18 +7379,14 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>37664.06410467719</v>
+        <v>38127.58363487636</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>sqrt</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>15</v>
       </c>
@@ -7467,12 +7396,12 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>38738.44583785938</v>
+        <v>39138.87645745221</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
@@ -7484,14 +7413,18 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>39229.44064888128</v>
+        <v>41013.47268592839</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sqrt</t>
+        </is>
+      </c>
       <c r="C5" t="n">
         <v>15</v>
       </c>
@@ -7501,7 +7434,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>40415.9440021121</v>
+        <v>41103.04833100144</v>
       </c>
     </row>
   </sheetData>
@@ -7589,7 +7522,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>34133.17503429761</v>
+        <v>34133.17503429762</v>
       </c>
     </row>
     <row r="4">
@@ -7610,7 +7543,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>34292.86315417191</v>
+        <v>34292.86315417192</v>
       </c>
     </row>
     <row r="5">
@@ -7631,7 +7564,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>34420.04770665281</v>
+        <v>34420.04770665283</v>
       </c>
     </row>
     <row r="6">
@@ -7652,7 +7585,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>34478.27029835433</v>
+        <v>34478.27029835435</v>
       </c>
     </row>
     <row r="7">
@@ -7694,7 +7627,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>34619.08061795308</v>
+        <v>34619.0806179531</v>
       </c>
     </row>
     <row r="9">
@@ -7715,7 +7648,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>34820.78889343506</v>
+        <v>34820.78889343508</v>
       </c>
     </row>
     <row r="10">
@@ -7736,7 +7669,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>35042.0987544189</v>
+        <v>35042.09875441891</v>
       </c>
     </row>
     <row r="11">
@@ -7778,7 +7711,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>35144.88985910764</v>
+        <v>35144.88985910766</v>
       </c>
     </row>
     <row r="13">
@@ -7799,7 +7732,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>35191.91948189725</v>
+        <v>35191.91948189727</v>
       </c>
     </row>
     <row r="14">
@@ -7820,7 +7753,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>35230.65999387588</v>
+        <v>35230.65999387589</v>
       </c>
     </row>
     <row r="15">
@@ -7862,7 +7795,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>35909.32973605605</v>
+        <v>35909.32973605607</v>
       </c>
     </row>
     <row r="17">
@@ -7883,7 +7816,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>36025.27151501396</v>
+        <v>36025.27151501397</v>
       </c>
     </row>
     <row r="18">
@@ -7904,7 +7837,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>36114.98207599313</v>
+        <v>36114.98207599315</v>
       </c>
     </row>
     <row r="19">
@@ -7925,7 +7858,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>36575.86373570783</v>
+        <v>36575.86373570785</v>
       </c>
     </row>
     <row r="20">
@@ -7946,7 +7879,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>36875.33557371929</v>
+        <v>36875.33557371931</v>
       </c>
     </row>
     <row r="21">
@@ -7967,7 +7900,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>36884.32689601757</v>
+        <v>36884.32689601758</v>
       </c>
     </row>
     <row r="22">
@@ -7988,7 +7921,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>37324.10807364617</v>
+        <v>37324.10807364619</v>
       </c>
     </row>
     <row r="23">
@@ -8009,7 +7942,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>37673.05623397124</v>
+        <v>37673.05623397126</v>
       </c>
     </row>
     <row r="24">
@@ -8030,7 +7963,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>37793.91708168892</v>
+        <v>37793.91708168895</v>
       </c>
     </row>
     <row r="25">
@@ -8051,7 +7984,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>38523.85249836884</v>
+        <v>38523.85249836886</v>
       </c>
     </row>
     <row r="26">
@@ -8072,7 +8005,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>39216.38518151857</v>
+        <v>39216.38518151858</v>
       </c>
     </row>
     <row r="27">
@@ -8093,7 +8026,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>39773.41866013689</v>
+        <v>39773.41866013691</v>
       </c>
     </row>
     <row r="28">
@@ -8114,7 +8047,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>39864.13621313719</v>
+        <v>39864.13621313721</v>
       </c>
     </row>
     <row r="29">
@@ -8135,7 +8068,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>40404.9404437202</v>
+        <v>40404.94044372023</v>
       </c>
     </row>
     <row r="30">
@@ -8156,7 +8089,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>40840.08519674537</v>
+        <v>40840.08519674539</v>
       </c>
     </row>
     <row r="31">
@@ -8177,7 +8110,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>41831.06485975582</v>
+        <v>41831.06485975585</v>
       </c>
     </row>
     <row r="32">
@@ -8198,7 +8131,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>41991.75313157144</v>
+        <v>41991.75313157147</v>
       </c>
     </row>
     <row r="33">
@@ -8219,7 +8152,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>42217.8070074708</v>
+        <v>42217.80700747082</v>
       </c>
     </row>
     <row r="34">
@@ -8240,7 +8173,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>42586.65503802924</v>
+        <v>42586.65503802925</v>
       </c>
     </row>
     <row r="35">
@@ -8261,7 +8194,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>42874.98372231896</v>
+        <v>42874.98372231898</v>
       </c>
     </row>
     <row r="36">
@@ -8282,7 +8215,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>42971.21122122814</v>
+        <v>42971.21122122816</v>
       </c>
     </row>
     <row r="37">
@@ -8303,7 +8236,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>42981.37204286241</v>
+        <v>42981.37204286244</v>
       </c>
     </row>
     <row r="38">
@@ -8324,7 +8257,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>44044.53225786884</v>
+        <v>44044.53225786886</v>
       </c>
     </row>
     <row r="39">
@@ -8345,7 +8278,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>44049.67434352594</v>
+        <v>44049.67434352595</v>
       </c>
     </row>
   </sheetData>
@@ -8418,7 +8351,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>35436.09586177427</v>
+        <v>35436.09586177426</v>
       </c>
     </row>
   </sheetData>
@@ -8515,7 +8448,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>27646.81273464491</v>
+        <v>27646.81273464492</v>
       </c>
     </row>
     <row r="3">
@@ -8551,7 +8484,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>27647.00486846996</v>
+        <v>27647.00486846997</v>
       </c>
     </row>
     <row r="4">
@@ -8623,7 +8556,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>27652.81472223818</v>
+        <v>27652.81472224246</v>
       </c>
     </row>
     <row r="6">
@@ -8659,7 +8592,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>27655.25242106362</v>
+        <v>27655.25242106292</v>
       </c>
     </row>
     <row r="7">
@@ -8695,7 +8628,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>27681.91334241445</v>
+        <v>27681.91334243699</v>
       </c>
     </row>
     <row r="8">
@@ -8731,7 +8664,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>27730.86374826047</v>
+        <v>27730.86374826048</v>
       </c>
     </row>
     <row r="9">
@@ -8767,7 +8700,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>28262.81985446589</v>
+        <v>28262.81985477017</v>
       </c>
     </row>
     <row r="10">
@@ -8803,7 +8736,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>30025.48645746997</v>
+        <v>31372.41068573633</v>
       </c>
     </row>
     <row r="11">
@@ -8839,7 +8772,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>33617.08911866674</v>
+        <v>34042.71300257614</v>
       </c>
     </row>
     <row r="12">
@@ -8875,7 +8808,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>35247.97990286242</v>
+        <v>34103.79819018038</v>
       </c>
     </row>
     <row r="13">
@@ -8911,7 +8844,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>36458.55637346413</v>
+        <v>38287.55485423729</v>
       </c>
     </row>
     <row r="14">
@@ -8947,7 +8880,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>41419.67275795194</v>
+        <v>41598.0472169337</v>
       </c>
     </row>
     <row r="15">
@@ -8983,7 +8916,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>45623.29172679084</v>
+        <v>45269.33597282472</v>
       </c>
     </row>
     <row r="16">
@@ -9019,7 +8952,7 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>49063.10757019669</v>
+        <v>49480.39266571088</v>
       </c>
     </row>
     <row r="17">
@@ -9055,7 +8988,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>58846.84965405006</v>
+        <v>58238.90492628535</v>
       </c>
     </row>
   </sheetData>
@@ -9109,7 +9042,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C2" t="n">
         <v>15</v>
@@ -9120,7 +9053,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>31193.84613159765</v>
+        <v>31354.90653674423</v>
       </c>
     </row>
     <row r="3">
@@ -9128,7 +9061,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C3" t="n">
         <v>15</v>
@@ -9139,7 +9072,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>31382.5109262373</v>
+        <v>31488.24450958332</v>
       </c>
     </row>
     <row r="4">
@@ -9147,7 +9080,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C4" t="n">
         <v>15</v>
@@ -9158,7 +9091,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>31709.20889621652</v>
+        <v>31721.58036541155</v>
       </c>
     </row>
     <row r="5">
@@ -9177,7 +9110,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>33785.1993596434</v>
+        <v>33382.54691485431</v>
       </c>
     </row>
     <row r="6">
@@ -9196,7 +9129,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>33814.36108078439</v>
+        <v>34031.33116432883</v>
       </c>
     </row>
     <row r="7">
@@ -9215,7 +9148,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>34091.69721106249</v>
+        <v>34165.51553438669</v>
       </c>
     </row>
   </sheetData>
@@ -9290,7 +9223,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>27612.34172955778</v>
+        <v>27612.34172955779</v>
       </c>
     </row>
     <row r="3">
@@ -9314,7 +9247,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>27612.34172955778</v>
+        <v>27612.34172955779</v>
       </c>
     </row>
     <row r="4">
@@ -9338,7 +9271,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>27612.34172955778</v>
+        <v>27612.34172955779</v>
       </c>
     </row>
     <row r="5">
@@ -9362,7 +9295,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>27619.18698795249</v>
+        <v>27619.1869879525</v>
       </c>
     </row>
     <row r="6">
@@ -9386,7 +9319,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>27619.18698795249</v>
+        <v>27619.1869879525</v>
       </c>
     </row>
     <row r="7">
@@ -9410,7 +9343,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>27619.18698795249</v>
+        <v>27619.1869879525</v>
       </c>
     </row>
     <row r="8">
@@ -9434,7 +9367,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>27632.8995964563</v>
+        <v>27632.89959645631</v>
       </c>
     </row>
     <row r="9">
@@ -9458,7 +9391,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>27632.8995964563</v>
+        <v>27632.89959645631</v>
       </c>
     </row>
     <row r="10">
@@ -9482,7 +9415,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>27632.8995964563</v>
+        <v>27632.89959645631</v>
       </c>
     </row>
     <row r="11">
@@ -9506,7 +9439,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>27646.64162404484</v>
+        <v>27646.64162404485</v>
       </c>
     </row>
     <row r="12">
@@ -9530,7 +9463,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>27646.64162404484</v>
+        <v>27646.64162404485</v>
       </c>
     </row>
     <row r="13">
@@ -9554,7 +9487,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>27646.64162404484</v>
+        <v>27646.64162404485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>